<commit_message>
csv data processing script and calcs added
</commit_message>
<xml_diff>
--- a/test_data_1.xlsx
+++ b/test_data_1.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Postgrad\6. Projects\electro-mech-stretcher\code\electromech-stretcher\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rel80.MECH2030\OneDrive - University of Canterbury\Postgrad\6. Projects\Electro-Mechanical Material Tester\6. Code\electromech-stretcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2838D958-38DD-460C-9E9D-A54648CE86EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -603,6 +602,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2806,6 +2806,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1249415087"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2818,6 +2819,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2849,6 +2851,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2856,7 +2859,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2936,6 +2938,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3819,6 +3822,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3826,7 +3830,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3924,6 +3927,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4787,6 +4791,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -4794,7 +4799,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -6915,20 +6919,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -6954,7 +6958,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>7324121.0999999996</v>
       </c>
@@ -6982,7 +6986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>6159364.0999999996</v>
       </c>
@@ -7010,7 +7014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6062177.2999999998</v>
       </c>
@@ -7038,7 +7042,7 @@
         <v>1.0085999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6079638.7000000002</v>
       </c>
@@ -7066,7 +7070,7 @@
         <v>1.0108999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6194161.7000000002</v>
       </c>
@@ -7094,7 +7098,7 @@
         <v>1.0131999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6293980.2999999998</v>
       </c>
@@ -7122,7 +7126,7 @@
         <v>1.0154999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6121245.7000000002</v>
       </c>
@@ -7150,7 +7154,7 @@
         <v>1.0188999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6147270.5999999996</v>
       </c>
@@ -7178,7 +7182,7 @@
         <v>1.0257999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5968666.7999999998</v>
       </c>
@@ -7206,7 +7210,7 @@
         <v>1.0281</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6054971.4000000004</v>
       </c>
@@ -7234,7 +7238,7 @@
         <v>1.0304</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6247193.2999999998</v>
       </c>
@@ -7262,7 +7266,7 @@
         <v>1.0326</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6348661.8999999901</v>
       </c>
@@ -7290,7 +7294,7 @@
         <v>1.0361</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6323702.1999999899</v>
       </c>
@@ -7318,7 +7322,7 @@
         <v>1.0428999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6270043.3999999901</v>
       </c>
@@ -7346,7 +7350,7 @@
         <v>1.0451999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6487956.2999999998</v>
       </c>
@@ -7374,7 +7378,7 @@
         <v>1.0474999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6822648.4000000004</v>
       </c>
@@ -7402,7 +7406,7 @@
         <v>1.0497999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6842031.2999999998</v>
       </c>
@@ -7430,7 +7434,7 @@
         <v>1.0528999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6863544.7000000002</v>
       </c>
@@ -7458,7 +7462,7 @@
         <v>1.0598000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6769177.5999999996</v>
       </c>
@@ -7486,7 +7490,7 @@
         <v>1.0619999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6758483.5999999996</v>
       </c>
@@ -7514,7 +7518,7 @@
         <v>1.0642</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6713493.4000000004</v>
       </c>
@@ -7542,7 +7546,7 @@
         <v>1.0665</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6808549.2000000002</v>
       </c>
@@ -7570,7 +7574,7 @@
         <v>1.0696999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6788581.4000000004</v>
       </c>
@@ -7598,7 +7602,7 @@
         <v>1.0762</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6685233.0999999996</v>
       </c>
@@ -7626,7 +7630,7 @@
         <v>1.0784</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6602165.7999999998</v>
       </c>
@@ -7654,7 +7658,7 @@
         <v>1.0807</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6497835.7999999998</v>
       </c>
@@ -7682,7 +7686,7 @@
         <v>1.0829</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6582845.5</v>
       </c>
@@ -7710,7 +7714,7 @@
         <v>1.0862000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6528519</v>
       </c>
@@ -7738,7 +7742,7 @@
         <v>1.0927</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6630050.2000000002</v>
       </c>
@@ -7766,7 +7770,7 @@
         <v>1.095</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6613131.9000000004</v>
       </c>
@@ -7794,7 +7798,7 @@
         <v>1.0972</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6713765</v>
       </c>
@@ -7822,7 +7826,7 @@
         <v>1.0994999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>6676836.5999999996</v>
       </c>
@@ -7850,7 +7854,7 @@
         <v>1.1026</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>6790899.7999999998</v>
       </c>
@@ -7878,7 +7882,7 @@
         <v>1.1091</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>6729116.6999999899</v>
       </c>
@@ -7906,7 +7910,7 @@
         <v>1.1113</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>6835493.7000000002</v>
       </c>
@@ -7934,7 +7938,7 @@
         <v>1.1135999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>6843681.4000000004</v>
       </c>
@@ -7962,7 +7966,7 @@
         <v>1.1159000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>6723707.0999999996</v>
       </c>
@@ -7990,7 +7994,7 @@
         <v>1.1191</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>6777887.4000000004</v>
       </c>
@@ -8018,7 +8022,7 @@
         <v>1.1259000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>6688679.3999999901</v>
       </c>
@@ -8046,7 +8050,7 @@
         <v>1.1281000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>6668565.5</v>
       </c>
@@ -8074,7 +8078,7 @@
         <v>1.1304000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6871982.8999999901</v>
       </c>
@@ -8102,7 +8106,7 @@
         <v>1.1326000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>6937609.5</v>
       </c>
@@ -8130,7 +8134,7 @@
         <v>1.1358999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>7013783.5999999996</v>
       </c>
@@ -8158,7 +8162,7 @@
         <v>1.1423000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>6995152.5999999996</v>
       </c>
@@ -8186,7 +8190,7 @@
         <v>1.1445000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>7223905.9000000004</v>
       </c>
@@ -8214,7 +8218,7 @@
         <v>1.1468</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>7189108.5</v>
       </c>
@@ -8242,7 +8246,7 @@
         <v>1.1491</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>7294065</v>
       </c>
@@ -8270,7 +8274,7 @@
         <v>1.1522999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>7217994.8999999901</v>
       </c>
@@ -8298,7 +8302,7 @@
         <v>1.1588000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>7271277.5</v>
       </c>
@@ -8326,7 +8330,7 @@
         <v>1.161</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>7069719</v>
       </c>
@@ -8354,7 +8358,7 @@
         <v>1.1633</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>7186685.5999999996</v>
       </c>
@@ -8382,7 +8386,7 @@
         <v>1.1655</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>7463311.7999999998</v>
       </c>
@@ -8410,7 +8414,7 @@
         <v>1.1686999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>7554086.0999999996</v>
       </c>
@@ -8438,7 +8442,7 @@
         <v>1.1755</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>7777868.4000000004</v>
       </c>
@@ -8466,7 +8470,7 @@
         <v>1.1778</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>7443427</v>
       </c>
@@ -8494,7 +8498,7 @@
         <v>1.1800000000000002</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>7400170.4000000004</v>
       </c>
@@ -8522,7 +8526,7 @@
         <v>1.1823000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>7663387.2999999998</v>
       </c>
@@ -8550,7 +8554,7 @@
         <v>1.1855</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>7880986.8999999901</v>
       </c>
@@ -8578,7 +8582,7 @@
         <v>1.1919999999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>7773043.5999999996</v>
       </c>
@@ -8606,7 +8610,7 @@
         <v>1.1942999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>7985525.8999999901</v>
       </c>
@@ -8634,7 +8638,7 @@
         <v>1.1964999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>8163398.1999999899</v>
       </c>
@@ -8662,7 +8666,7 @@
         <v>1.1987999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>8274808.9999999898</v>
       </c>
@@ -8690,7 +8694,7 @@
         <v>1.2022999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>8567601.5999999996</v>
       </c>
@@ -8718,7 +8722,7 @@
         <v>1.2092000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>8517786.6999999993</v>
       </c>
@@ -8746,7 +8750,7 @@
         <v>1.2114</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>8389290.5</v>
       </c>
@@ -8774,7 +8778,7 @@
         <v>1.2137</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>8263843.4000000004</v>
       </c>
@@ -8802,7 +8806,7 @@
         <v>1.2159</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>8479730.1999999993</v>
       </c>
@@ -8830,7 +8834,7 @@
         <v>1.2190999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>8477453.5999999996</v>
       </c>
@@ -8858,7 +8862,7 @@
         <v>1.2256</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>8696369.1999999993</v>
       </c>
@@ -8886,7 +8890,7 @@
         <v>1.2279</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>8650209.4000000004</v>
       </c>
@@ -8914,7 +8918,7 @@
         <v>1.2301</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>9081105.9000000004</v>
       </c>
@@ -8942,7 +8946,7 @@
         <v>1.2324999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>9520044.0999999996</v>
       </c>
@@ -8970,7 +8974,7 @@
         <v>1.2356</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>9647392</v>
       </c>
@@ -8998,7 +9002,7 @@
         <v>1.2423999999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>9518331.3999999892</v>
       </c>
@@ -9026,7 +9030,7 @@
         <v>1.2445999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>9854443.2999999896</v>
       </c>
@@ -9054,7 +9058,7 @@
         <v>1.2468999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>9430000.4000000004</v>
       </c>
@@ -9082,7 +9086,7 @@
         <v>1.2492000000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>9508639.9000000004</v>
       </c>
@@ -9110,7 +9114,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>9741278.0999999996</v>
       </c>
@@ -9138,7 +9142,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>9925563.4000000004</v>
       </c>
@@ -9166,7 +9170,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>10045871</v>
       </c>
@@ -9194,7 +9198,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>9989582</v>
       </c>
@@ -9222,7 +9226,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>9832909</v>
       </c>
@@ -9250,7 +9254,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>9551186.8999999892</v>
       </c>
@@ -9278,7 +9282,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>9534226.1999999993</v>
       </c>
@@ -9306,7 +9310,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>9604531.6999999993</v>
       </c>
@@ -9334,7 +9338,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>9444037.0999999996</v>
       </c>
@@ -9362,7 +9366,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>9736912.8000000007</v>
       </c>
@@ -9390,7 +9394,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>9829316.5</v>
       </c>
@@ -9418,7 +9422,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>9868730.5</v>
       </c>
@@ -9446,7 +9450,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>9875372.4000000004</v>
       </c>
@@ -9474,7 +9478,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>9959107.5999999996</v>
       </c>
@@ -9502,7 +9506,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>9776556.5</v>
       </c>
@@ -9530,7 +9534,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>9664895.0999999996</v>
       </c>
@@ -9558,7 +9562,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>9652780.8000000007</v>
       </c>
@@ -9586,7 +9590,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>9555009.1999999993</v>
       </c>
@@ -9614,7 +9618,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>9540053.5999999996</v>
       </c>
@@ -9642,7 +9646,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>9449968.9000000004</v>
       </c>
@@ -9670,7 +9674,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>9551834.4000000004</v>
       </c>
@@ -9698,7 +9702,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>9553171.0999999996</v>
       </c>
@@ -9726,7 +9730,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>9570799.5999999996</v>
       </c>

</xml_diff>